<commit_message>
added structure to project
</commit_message>
<xml_diff>
--- a/meting WV py.xlsx
+++ b/meting WV py.xlsx
@@ -965,27 +965,27 @@
       </c>
     </row>
     <row r="18">
-      <c r="F18" t="n">
+      <c r="F18" s="0" t="n">
         <v>262144</v>
       </c>
     </row>
     <row r="19">
-      <c r="F19" t="n">
+      <c r="F19" s="0" t="n">
         <v>524288</v>
       </c>
     </row>
     <row r="20">
-      <c r="F20" t="n">
+      <c r="F20" s="0" t="n">
         <v>1048576</v>
       </c>
     </row>
     <row r="21">
-      <c r="F21" t="n">
+      <c r="F21" s="0" t="n">
         <v>2097152</v>
       </c>
     </row>
     <row r="22">
-      <c r="F22" t="n">
+      <c r="F22" s="0" t="n">
         <v>4194304</v>
       </c>
     </row>

</xml_diff>